<commit_message>
import des donnees de user
</commit_message>
<xml_diff>
--- a/userImport.xlsx
+++ b/userImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caign\OneDrive\Documents\SkiUTC\server-SkiUt-P25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824D105F-CBA6-4D13-87E0-39FC2B91FF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5532C3B3-2486-4A7A-BCF3-3889A01C55EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3032" uniqueCount="1390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3048" uniqueCount="1398">
   <si>
     <t>rbaudoin</t>
   </si>
@@ -4195,6 +4195,30 @@
   </si>
   <si>
     <t>adventur</t>
+  </si>
+  <si>
+    <t>Raian</t>
+  </si>
+  <si>
+    <t>Husein</t>
+  </si>
+  <si>
+    <t>rahusein</t>
+  </si>
+  <si>
+    <t>yan.husein@etu.utc.fr</t>
+  </si>
+  <si>
+    <t>Aymeric</t>
+  </si>
+  <si>
+    <t>Forget</t>
+  </si>
+  <si>
+    <t>aymeric841@gmail.com</t>
+  </si>
+  <si>
+    <t>ayforget</t>
   </si>
 </sst>
 </file>
@@ -4253,7 +4277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -4298,12 +4322,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4327,22 +4360,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4639,14 +4675,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A1DB05-A62D-4851-AF9A-0162B7AA0295}">
-  <dimension ref="A1:J379"/>
+  <dimension ref="A1:J381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A369" workbookViewId="0">
-      <selection activeCell="H375" sqref="H375"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="5" max="5" width="44.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.90625" style="12"/>
   </cols>
   <sheetData>
@@ -5482,35 +5519,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
+    <row r="27" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="17">
         <v>334852</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="10">
-        <v>25</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J27" s="4" t="s">
+      <c r="F27" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="19">
+        <v>52</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7102,7 +7139,7 @@
         <v>4</v>
       </c>
       <c r="G77" s="10">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>4</v>
@@ -7166,7 +7203,7 @@
         <v>4</v>
       </c>
       <c r="G79" s="10">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>4</v>
@@ -9418,35 +9455,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A150" s="2">
+    <row r="150" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="17">
         <v>316633</v>
       </c>
-      <c r="B150" s="5" t="s">
+      <c r="B150" s="18" t="s">
         <v>562</v>
       </c>
-      <c r="C150" s="5" t="s">
+      <c r="C150" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="D150" s="5" t="s">
+      <c r="D150" s="18" t="s">
         <v>563</v>
       </c>
-      <c r="E150" s="5" t="s">
+      <c r="E150" s="18" t="s">
         <v>564</v>
       </c>
-      <c r="F150" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G150" s="11">
+      <c r="F150" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G150" s="19">
         <v>44</v>
       </c>
-      <c r="H150" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I150" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J150" s="6" t="s">
+      <c r="H150" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I150" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J150" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -9822,7 +9859,7 @@
         <v>4</v>
       </c>
       <c r="G162" s="11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H162" s="5" t="s">
         <v>4</v>
@@ -12638,7 +12675,7 @@
         <v>4</v>
       </c>
       <c r="G250" s="11">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="H250" s="5" t="s">
         <v>4</v>
@@ -14206,7 +14243,7 @@
         <v>4</v>
       </c>
       <c r="G299" s="10">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="H299" s="3" t="s">
         <v>4</v>
@@ -15102,7 +15139,7 @@
         <v>4</v>
       </c>
       <c r="G327" s="10">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="H327" s="3" t="s">
         <v>4</v>
@@ -16776,13 +16813,77 @@
       </c>
       <c r="J379" s="4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="380" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A380">
+        <v>119348</v>
+      </c>
+      <c r="B380" s="13" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C380" s="13" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D380" s="13" t="s">
+        <v>1391</v>
+      </c>
+      <c r="E380" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F380" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G380" s="12">
+        <v>6</v>
+      </c>
+      <c r="H380" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I380" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J380" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="381" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A381">
+        <v>97187</v>
+      </c>
+      <c r="B381" s="15" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C381" s="15" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D381" s="15" t="s">
+        <v>1395</v>
+      </c>
+      <c r="E381" t="s">
+        <v>1396</v>
+      </c>
+      <c r="F381" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G381" s="12">
+        <v>25</v>
+      </c>
+      <c r="H381" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I381" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="J381" s="16" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A379">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B379">
+  <conditionalFormatting sqref="B1:B381">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>